<commit_message>
Excel data format - done
Allure setup - done

Done Manage Client Page
</commit_message>
<xml_diff>
--- a/src/main/java/main_HRM_anhtester/datatest/excel/LoginPage.xlsx
+++ b/src/main/java/main_HRM_anhtester/datatest/excel/LoginPage.xlsx
@@ -211,175 +211,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -549,7 +549,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -573,16 +573,16 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -591,78 +591,78 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -673,14 +673,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1222,7 +1219,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="2"/>
@@ -1236,21 +1233,21 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" ht="27" customHeight="1" spans="1:3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>123456</v>
       </c>
     </row>

</xml_diff>